<commit_message>
Marked my name for da rows
</commit_message>
<xml_diff>
--- a/Data/ModelPerformances.xlsx
+++ b/Data/ModelPerformances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Daniel\Biola-Lawrence-Livermore-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D969CC-572F-48CF-A700-D3396585AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA47C24B-D302-4C7C-A3AF-34D38316976E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>1. Split data based on percentage</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>5. Repeat (1-4) 3 times, average</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Final analysis and graphs</t>
   </si>
 </sst>
 </file>
@@ -175,12 +181,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
@@ -463,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:T32"/>
+  <dimension ref="A7:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,14 +480,7 @@
     <col min="18" max="18" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -494,25 +492,21 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="4"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="4"/>
       <c r="R7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2">
         <v>1</v>
@@ -529,12 +523,10 @@
       <c r="F8" s="2">
         <v>0.25</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>0.1</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="H8" s="5"/>
       <c r="K8" s="2">
         <v>1</v>
       </c>
@@ -553,12 +545,9 @@
       <c r="P8" s="2">
         <v>0.1</v>
       </c>
-      <c r="Q8" s="4"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -568,21 +557,16 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="H9" s="5"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="4"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -592,21 +576,16 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="H10" s="5"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="4"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -616,21 +595,16 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="H11" s="5"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="4"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -640,21 +614,16 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="H12" s="5"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="4"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -664,21 +633,16 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="H13" s="5"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="4"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -688,21 +652,16 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="H14" s="5"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="4"/>
       <c r="R14" s="1"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -712,21 +671,16 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="H15" s="5"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="4"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -736,21 +690,16 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="H16" s="5"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="4"/>
       <c r="R16" s="1"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -760,21 +709,16 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="H17" s="5"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="4"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -784,21 +728,16 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="H18" s="5"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-      <c r="Q18" s="4"/>
       <c r="R18" s="1"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -808,21 +747,18 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="H19" s="5"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -832,21 +768,18 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="H20" s="5"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -856,21 +789,18 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="H21" s="5"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -880,21 +810,18 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="H22" s="5"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -904,21 +831,18 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="H23" s="5"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -928,21 +852,18 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
+      <c r="H24" s="5"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -952,63 +873,44 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="H25" s="5"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-      <c r="Q25" s="4"/>
       <c r="R25" s="1"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="Q27" s="4"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R26" t="s">
+        <v>26</v>
+      </c>
+      <c r="S26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="Q28" s="4"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
-      <c r="H29" s="4"/>
-      <c r="Q29" s="4"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
-      <c r="Q30" s="4"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
-      <c r="Q31" s="4"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Min model size ran
</commit_message>
<xml_diff>
--- a/Data/ModelPerformances.xlsx
+++ b/Data/ModelPerformances.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Daniel\Biola-Lawrence-Livermore-Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel\Documents\GitHub\Biola-Lawrence-Livermore-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C1D3D9-75CC-4F12-9AA2-44BAC81E8116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC034847-C830-4EAD-948F-A70EDF3693F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>1. Split data based on percentage</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Note class should be accuracy, regr should be mean squared error</t>
+  </si>
+  <si>
+    <t>63 params</t>
   </si>
 </sst>
 </file>
@@ -198,14 +201,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,7 +498,7 @@
   <dimension ref="A6:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,209 +583,235 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="3"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
       <c r="H9" s="5"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="3"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
       <c r="H10" s="5"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="3"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="5"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="3"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="5"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="3"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
       <c r="H13" s="5"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="3"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="5"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="3"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
       <c r="H15" s="5"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="3"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
       <c r="H16" s="5"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="3"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="5"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
       <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="3"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="5"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="5"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
+      <c r="B19" s="7">
+        <v>0.92025518417358398</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.93033401171366303</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0.92022582888603199</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.96416300535202004</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0.95139908790588301</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.97539975245793598</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="7">
+        <v>0.88039215405782001</v>
+      </c>
+      <c r="L19" s="7">
+        <v>0.89313725630442298</v>
+      </c>
+      <c r="M19" s="7">
+        <v>0.86764705181121804</v>
+      </c>
+      <c r="N19" s="7">
+        <v>0.88725491364796905</v>
+      </c>
+      <c r="O19" s="7">
+        <v>0.87352943420410101</v>
+      </c>
+      <c r="P19" s="7">
+        <v>0.83627450466155995</v>
+      </c>
       <c r="R19" s="1" t="s">
         <v>24</v>
       </c>
@@ -785,19 +820,19 @@
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="3"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
       <c r="H20" s="5"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
       <c r="R20" s="1" t="s">
         <v>24</v>
       </c>
@@ -806,41 +841,41 @@
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="7">
         <v>0.64961352944373996</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="7">
         <v>0.67252896229425996</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="7">
         <v>0.68360334634780795</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="7">
         <v>0.68237604697545295</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="7">
         <v>0.673785001039505</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="8">
         <v>0.68265682458877497</v>
       </c>
       <c r="H21" s="5"/>
-      <c r="K21" s="1">
+      <c r="K21" s="7">
         <v>0.64558824896812395</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L21" s="7">
         <v>0.68235294024149495</v>
       </c>
-      <c r="M21" s="1">
+      <c r="M21" s="7">
         <v>0.68088233470916704</v>
       </c>
-      <c r="N21" s="1">
+      <c r="N21" s="7">
         <v>0.66862744092941195</v>
       </c>
-      <c r="O21" s="1">
+      <c r="O21" s="7">
         <v>0.67205882072448697</v>
       </c>
-      <c r="P21" s="1">
+      <c r="P21" s="7">
         <v>0.65294118722279804</v>
       </c>
       <c r="R21" s="1" t="s">
@@ -851,19 +886,43 @@
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="3"/>
+      <c r="B22" s="7">
+        <v>0.812457581361134</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.72090607881545998</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0.80801308155059803</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0.619081750512123</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.32622307538986201</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.29697552323341297</v>
+      </c>
       <c r="H22" s="5"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="K22" s="7">
+        <v>2.8074042797088601</v>
+      </c>
+      <c r="L22" s="7">
+        <v>3.0053186416625901</v>
+      </c>
+      <c r="M22" s="7">
+        <v>2.9003276824951101</v>
+      </c>
+      <c r="N22" s="7">
+        <v>3.4158694744110099</v>
+      </c>
+      <c r="O22" s="7">
+        <v>3.3557066917419398</v>
+      </c>
+      <c r="P22" s="7">
+        <v>4.5839817523956299</v>
+      </c>
       <c r="R22" s="1" t="s">
         <v>24</v>
       </c>
@@ -872,19 +931,19 @@
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="3"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8"/>
       <c r="H23" s="5"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
       <c r="R23" s="1" t="s">
         <v>24</v>
       </c>
@@ -893,41 +952,41 @@
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="7">
         <v>6.8464806079864502</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="7">
         <v>7.5379015604654898</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="7">
         <v>6.7218438784281398</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="7">
         <v>6.0046401023864702</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="7">
         <v>5.7922210693359304</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="8">
         <v>3.9683539072672498</v>
       </c>
       <c r="H24" s="5"/>
-      <c r="K24" s="1">
+      <c r="K24" s="7">
         <v>9.1825590133666992</v>
       </c>
-      <c r="L24" s="1">
+      <c r="L24" s="7">
         <v>8.7918961842854806</v>
       </c>
-      <c r="M24" s="1">
+      <c r="M24" s="7">
         <v>8.0945396423339808</v>
       </c>
-      <c r="N24" s="1">
+      <c r="N24" s="7">
         <v>9.0815939903259206</v>
       </c>
-      <c r="O24" s="1">
+      <c r="O24" s="7">
         <v>9.2357060114542602</v>
       </c>
-      <c r="P24" s="1">
+      <c r="P24" s="7">
         <v>10.9094778696695</v>
       </c>
       <c r="R24" s="1" t="s">
@@ -938,19 +997,19 @@
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="3"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
       <c r="H25" s="5"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -991,6 +1050,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modification of table so easy to export
</commit_message>
<xml_diff>
--- a/Data/ModelPerformances.xlsx
+++ b/Data/ModelPerformances.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel\Documents\GitHub\Biola-Lawrence-Livermore-Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Daniel\Biola-Lawrence-Livermore-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC034847-C830-4EAD-948F-A70EDF3693F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48048822-8261-4287-ACA2-F4119406B43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Exporatable" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
   <si>
     <t>1. Split data based on percentage</t>
   </si>
@@ -75,15 +76,9 @@
     <t>Min Input Space NN:</t>
   </si>
   <si>
-    <t>Med Input Space NN:</t>
-  </si>
-  <si>
     <t>Min Input Space NN Regr.:</t>
   </si>
   <si>
-    <t>Med Input Space NN Regr.:</t>
-  </si>
-  <si>
     <t>Aggregation</t>
   </si>
   <si>
@@ -118,14 +113,40 @@
   </si>
   <si>
     <t>63 params</t>
+  </si>
+  <si>
+    <t>Train: Accuracy:</t>
+  </si>
+  <si>
+    <t>Train: Regression</t>
+  </si>
+  <si>
+    <t>Val: Regression</t>
+  </si>
+  <si>
+    <t>Val: Accuracy:</t>
+  </si>
+  <si>
+    <t>Just Docking/Fusion NN</t>
+  </si>
+  <si>
+    <t>Min Input Space NN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -201,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -215,6 +236,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A6:S32"/>
+  <dimension ref="A6:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +535,7 @@
   <sheetData>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -526,7 +552,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="5"/>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -535,7 +561,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="R7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -792,7 +818,7 @@
         <v>0.97539975245793598</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K19" s="7">
         <v>0.88039215405782001</v>
@@ -813,123 +839,147 @@
         <v>0.83627450466155995</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0.64961352944373996</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.67252896229425996</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.68360334634780795</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.68237604697545295</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.673785001039505</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.68265682458877497</v>
+      </c>
       <c r="H20" s="5"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
+      <c r="K20" s="7">
+        <v>0.64558824896812395</v>
+      </c>
+      <c r="L20" s="7">
+        <v>0.68235294024149495</v>
+      </c>
+      <c r="M20" s="7">
+        <v>0.68088233470916704</v>
+      </c>
+      <c r="N20" s="7">
+        <v>0.66862744092941195</v>
+      </c>
+      <c r="O20" s="7">
+        <v>0.67205882072448697</v>
+      </c>
+      <c r="P20" s="7">
+        <v>0.65294118722279804</v>
+      </c>
       <c r="R20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B21" s="7">
-        <v>0.64961352944373996</v>
+        <v>0.812457581361134</v>
       </c>
       <c r="C21" s="7">
-        <v>0.67252896229425996</v>
+        <v>0.72090607881545998</v>
       </c>
       <c r="D21" s="7">
-        <v>0.68360334634780795</v>
+        <v>0.80801308155059803</v>
       </c>
       <c r="E21" s="7">
-        <v>0.68237604697545295</v>
+        <v>0.619081750512123</v>
       </c>
       <c r="F21" s="7">
-        <v>0.673785001039505</v>
+        <v>0.32622307538986201</v>
       </c>
       <c r="G21" s="8">
-        <v>0.68265682458877497</v>
+        <v>0.29697552323341297</v>
       </c>
       <c r="H21" s="5"/>
       <c r="K21" s="7">
-        <v>0.64558824896812395</v>
+        <v>2.8074042797088601</v>
       </c>
       <c r="L21" s="7">
-        <v>0.68235294024149495</v>
+        <v>3.0053186416625901</v>
       </c>
       <c r="M21" s="7">
-        <v>0.68088233470916704</v>
+        <v>2.9003276824951101</v>
       </c>
       <c r="N21" s="7">
-        <v>0.66862744092941195</v>
+        <v>3.4158694744110099</v>
       </c>
       <c r="O21" s="7">
-        <v>0.67205882072448697</v>
+        <v>3.3557066917419398</v>
       </c>
       <c r="P21" s="7">
-        <v>0.65294118722279804</v>
+        <v>4.5839817523956299</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B22" s="7">
-        <v>0.812457581361134</v>
+        <v>6.8464806079864502</v>
       </c>
       <c r="C22" s="7">
-        <v>0.72090607881545998</v>
+        <v>7.5379015604654898</v>
       </c>
       <c r="D22" s="7">
-        <v>0.80801308155059803</v>
+        <v>6.7218438784281398</v>
       </c>
       <c r="E22" s="7">
-        <v>0.619081750512123</v>
+        <v>6.0046401023864702</v>
       </c>
       <c r="F22" s="7">
-        <v>0.32622307538986201</v>
+        <v>5.7922210693359304</v>
       </c>
       <c r="G22" s="8">
-        <v>0.29697552323341297</v>
+        <v>3.9683539072672498</v>
       </c>
       <c r="H22" s="5"/>
       <c r="K22" s="7">
-        <v>2.8074042797088601</v>
+        <v>9.1825590133666992</v>
       </c>
       <c r="L22" s="7">
-        <v>3.0053186416625901</v>
+        <v>8.7918961842854806</v>
       </c>
       <c r="M22" s="7">
-        <v>2.9003276824951101</v>
+        <v>8.0945396423339808</v>
       </c>
       <c r="N22" s="7">
-        <v>3.4158694744110099</v>
+        <v>9.0815939903259206</v>
       </c>
       <c r="O22" s="7">
-        <v>3.3557066917419398</v>
+        <v>9.2357060114542602</v>
       </c>
       <c r="P22" s="7">
-        <v>4.5839817523956299</v>
+        <v>10.9094778696695</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -944,112 +994,296 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
-      <c r="R23" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="R23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="7">
-        <v>6.8464806079864502</v>
-      </c>
-      <c r="C24" s="7">
-        <v>7.5379015604654898</v>
-      </c>
-      <c r="D24" s="7">
-        <v>6.7218438784281398</v>
-      </c>
-      <c r="E24" s="7">
-        <v>6.0046401023864702</v>
-      </c>
-      <c r="F24" s="7">
-        <v>5.7922210693359304</v>
-      </c>
-      <c r="G24" s="8">
-        <v>3.9683539072672498</v>
-      </c>
-      <c r="H24" s="5"/>
-      <c r="K24" s="7">
-        <v>9.1825590133666992</v>
-      </c>
-      <c r="L24" s="7">
-        <v>8.7918961842854806</v>
-      </c>
-      <c r="M24" s="7">
-        <v>8.0945396423339808</v>
-      </c>
-      <c r="N24" s="7">
-        <v>9.0815939903259206</v>
-      </c>
-      <c r="O24" s="7">
-        <v>9.2357060114542602</v>
-      </c>
-      <c r="P24" s="7">
-        <v>10.9094778696695</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="5"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="R25" s="1"/>
+      <c r="A24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R24" t="s">
+        <v>22</v>
+      </c>
+      <c r="S24" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="R26" t="s">
-        <v>24</v>
-      </c>
-      <c r="S26" t="s">
-        <v>25</v>
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D50979C-CACD-45CA-A395-10DC3E8DA3B3}">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="13">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="D1" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E1" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="F1" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="13">
+        <v>1</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="F21" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="13">
+        <v>1</v>
+      </c>
+      <c r="C28" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="F28" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added the Non PCA data to the table
</commit_message>
<xml_diff>
--- a/Data/ModelPerformances.xlsx
+++ b/Data/ModelPerformances.xlsx
@@ -5,28 +5,39 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Daniel\Biola-Lawrence-Livermore-Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesto\Documents\GitHub\Biola-Lawrence-Livermore-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48048822-8261-4287-ACA2-F4119406B43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830122BE-10CA-4DF8-B55D-633EEDFCB25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Data" sheetId="1" r:id="rId1"/>
     <sheet name="Exporatable" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>1. Split data based on percentage</t>
   </si>
@@ -131,13 +142,16 @@
   </si>
   <si>
     <t>Min Input Space NN</t>
+  </si>
+  <si>
+    <t>Jesse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +163,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -222,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -241,6 +262,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,22 +547,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A6:S30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="18" max="18" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" customWidth="1"/>
+    <col min="18" max="18" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -564,7 +588,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2">
         <v>1</v>
@@ -605,26 +629,56 @@
       </c>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
+      <c r="B9" s="7">
+        <v>0.97791681687037102</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.98050443331400505</v>
+      </c>
+      <c r="D9" s="7">
+        <f>(0.981132060289382 + 0.978257079919179)/2</f>
+        <v>0.97969457010428052</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.98355424404144198</v>
+      </c>
+      <c r="F9" s="7">
+        <f>(0.97914108633995 + 0.990791896979014)/2</f>
+        <v>0.98496649165948202</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.99015988906224495</v>
+      </c>
       <c r="H9" s="5"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K9" s="7">
+        <v>0.90392156442006399</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.90686275561650598</v>
+      </c>
+      <c r="M9" s="14">
+        <f>(0.911764681339263 + 0.901960770289103)/2</f>
+        <v>0.90686272581418303</v>
+      </c>
+      <c r="N9" s="7">
+        <v>0.89411763350168805</v>
+      </c>
+      <c r="O9" s="7">
+        <f>(0.907352954149246 + 0.877450982729593) /2</f>
+        <v>0.89240196843941955</v>
+      </c>
+      <c r="P9" s="7">
+        <v>0.87941175699233998</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -643,7 +697,7 @@
       <c r="P10" s="7"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -662,7 +716,7 @@
       <c r="P11" s="7"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -681,7 +735,7 @@
       <c r="P12" s="7"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -700,7 +754,7 @@
       <c r="P13" s="7"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -719,7 +773,7 @@
       <c r="P14" s="7"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -738,7 +792,7 @@
       <c r="P15" s="7"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -757,7 +811,7 @@
       <c r="P16" s="7"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -776,7 +830,7 @@
       <c r="P17" s="7"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -795,7 +849,7 @@
       <c r="P18" s="7"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -842,7 +896,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -887,7 +941,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -932,7 +986,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -977,7 +1031,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -996,7 +1050,7 @@
       <c r="P23" s="7"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1007,27 +1061,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1042,17 +1096,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D50979C-CACD-45CA-A395-10DC3E8DA3B3}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="17.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -1072,52 +1126,52 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>32</v>
       </c>
@@ -1137,52 +1191,52 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -1202,37 +1256,37 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1252,32 +1306,32 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
soft margin with and w/o pca
</commit_message>
<xml_diff>
--- a/Data/ModelPerformances.xlsx
+++ b/Data/ModelPerformances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesto\Documents\GitHub\Biola-Lawrence-Livermore-Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\Biola-Lawrence-Livermore-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830122BE-10CA-4DF8-B55D-633EEDFCB25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2A76B7-7854-41F1-91FD-A51323E3E2B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23258" windowHeight="12578" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Data" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>1. Split data based on percentage</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Jesse</t>
+  </si>
+  <si>
+    <t>Tim</t>
   </si>
 </sst>
 </file>
@@ -548,21 +551,21 @@
   <dimension ref="A6:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.109375" customWidth="1"/>
-    <col min="18" max="18" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.1328125" customWidth="1"/>
+    <col min="18" max="18" width="27.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -588,7 +591,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="2">
         <v>1</v>
@@ -629,7 +632,7 @@
       </c>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -678,7 +681,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -697,7 +700,7 @@
       <c r="P10" s="7"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -716,7 +719,7 @@
       <c r="P11" s="7"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -735,7 +738,7 @@
       <c r="P12" s="7"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -754,7 +757,7 @@
       <c r="P13" s="7"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -773,7 +776,7 @@
       <c r="P14" s="7"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -792,7 +795,7 @@
       <c r="P15" s="7"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -811,45 +814,97 @@
       <c r="P16" s="7"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
+      <c r="B17" s="7">
+        <v>0.96613899999999997</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.96605300000000005</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0.965144</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.96391700000000002</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.95434399999999997</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0.95571899999999999</v>
+      </c>
       <c r="H17" s="5"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K17" s="7">
+        <v>0.92058799999999996</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0.91176400000000002</v>
+      </c>
+      <c r="M17" s="7">
+        <v>0.90882300000000005</v>
+      </c>
+      <c r="N17" s="7">
+        <v>0.89705800000000002</v>
+      </c>
+      <c r="O17" s="7">
+        <v>0.88235200000000003</v>
+      </c>
+      <c r="P17" s="7">
+        <v>0.86176399999999997</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
+      <c r="B18" s="7">
+        <v>0.95362499999999994</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.95460100000000003</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0.95238</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0.94992600000000005</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0.94403499999999996</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.96309900000000004</v>
+      </c>
       <c r="H18" s="5"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="R18" s="1"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K18" s="7">
+        <v>0.91470499999999999</v>
+      </c>
+      <c r="L18" s="7">
+        <v>0.90294099999999999</v>
+      </c>
+      <c r="M18" s="7">
+        <v>0.90588199999999997</v>
+      </c>
+      <c r="N18" s="7">
+        <v>0.87646999999999997</v>
+      </c>
+      <c r="O18" s="7">
+        <v>0.888235</v>
+      </c>
+      <c r="P18" s="7">
+        <v>0.83529399999999998</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -896,7 +951,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -941,7 +996,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -986,7 +1041,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1031,7 +1086,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1050,7 +1105,7 @@
       <c r="P23" s="7"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1061,27 +1116,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1100,13 +1155,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.109375" style="10"/>
+    <col min="2" max="16384" width="9.1328125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -1126,52 +1181,52 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>32</v>
       </c>
@@ -1191,52 +1246,52 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -1256,37 +1311,37 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1306,32 +1361,32 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="10" t="s">
         <v>33</v>
       </c>

</xml_diff>